<commit_message>
Added pydantic data contract AbsenteeismSchema
</commit_message>
<xml_diff>
--- a/data/output/consolidated_absenteeism_data.xlsx
+++ b/data/output/consolidated_absenteeism_data.xlsx
@@ -497,7 +497,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>45094</v>
+        <v>25568.8755219213</v>
       </c>
       <c r="G2" t="n">
         <v>8675.889999999999</v>
@@ -526,7 +526,7 @@
         <v>4</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>45090</v>
+        <v>25568.875521875</v>
       </c>
       <c r="G3" t="n">
         <v>9222.18</v>
@@ -555,7 +555,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>45091</v>
+        <v>25568.87552188657</v>
       </c>
       <c r="G4" t="n">
         <v>5703.94</v>
@@ -584,7 +584,7 @@
         <v>7</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>45105</v>
+        <v>25568.87552204861</v>
       </c>
       <c r="G5" t="n">
         <v>10882.03</v>
@@ -613,7 +613,7 @@
         <v>2</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>45095</v>
+        <v>25568.87552193287</v>
       </c>
       <c r="G6" t="n">
         <v>12436.01</v>
@@ -642,7 +642,7 @@
         <v>8</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>45101</v>
+        <v>25568.87552200232</v>
       </c>
       <c r="G7" t="n">
         <v>5203.48</v>
@@ -671,7 +671,7 @@
         <v>4</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>45079</v>
+        <v>25568.87552174769</v>
       </c>
       <c r="G8" t="n">
         <v>7933.98</v>
@@ -700,7 +700,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>45099</v>
+        <v>25568.87552197917</v>
       </c>
       <c r="G9" t="n">
         <v>4297.17</v>
@@ -729,7 +729,7 @@
         <v>5</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>45086</v>
+        <v>25568.8755218287</v>
       </c>
       <c r="G10" t="n">
         <v>6403.86</v>
@@ -758,7 +758,7 @@
         <v>8</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>45078</v>
+        <v>25568.87552173611</v>
       </c>
       <c r="G11" t="n">
         <v>7977.81</v>

</xml_diff>